<commit_message>
sua lai cau truc thu muc
</commit_message>
<xml_diff>
--- a/apartmentManage/Data/apartments.xlsx
+++ b/apartmentManage/Data/apartments.xlsx
@@ -12,30 +12,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>apartment_id</t>
   </si>
   <si>
+    <t>apartmentIndex</t>
+  </si>
+  <si>
     <t>floor</t>
   </si>
   <si>
     <t>building</t>
   </si>
   <si>
+    <t>num_rooms</t>
+  </si>
+  <si>
     <t>status</t>
   </si>
   <si>
     <t>area</t>
   </si>
   <si>
+    <t>rent_price</t>
+  </si>
+  <si>
     <t>purchase_price</t>
   </si>
   <si>
-    <t>rental_price</t>
-  </si>
-  <si>
-    <t>num_rooms</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Đã thuê</t>
+  </si>
+  <si>
+    <t>55.00</t>
+  </si>
+  <si>
+    <t>5200000.00</t>
+  </si>
+  <si>
+    <t>4000000000.00</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Đã bán</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>6000000.00</t>
+  </si>
+  <si>
+    <t>5500000000.00</t>
   </si>
 </sst>
 </file>
@@ -80,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -111,6 +159,67 @@
       <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>